<commit_message>
CDF AD & CDF CH Update
</commit_message>
<xml_diff>
--- a/ccbhc_measurements/dashboard/excel files/CDF_AD_sub_1.xlsx
+++ b/ccbhc_measurements/dashboard/excel files/CDF_AD_sub_1.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -536,7 +532,7 @@
         </is>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -566,7 +562,7 @@
         </is>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -645,20 +641,14 @@
           <t>67362</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>46284</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>45313</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Positive screening without follow-up</t>
+          <t>No screening recorded</t>
         </is>
       </c>
       <c r="H7" t="b">
@@ -681,18 +671,14 @@
           <t>64340</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>77375</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Negative screening</t>
+          <t>No screening recorded</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -745,22 +731,18 @@
           <t>38189</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>88584</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Negative screening</t>
+          <t>No screening recorded</t>
         </is>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -781,22 +763,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>43299</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>45298</v>
-      </c>
+          <t>22777</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Positive screening without follow-up</t>
+          <t>Negative screening</t>
         </is>
       </c>
       <c r="H11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -815,20 +795,14 @@
           <t>93205</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>95272</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>45299</v>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="b">
         <v>0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Positive screening without follow-up</t>
+          <t>No screening recorded</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -851,18 +825,14 @@
           <t>26431</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>77654</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Negative screening</t>
+          <t>No screening recorded</t>
         </is>
       </c>
       <c r="H13" t="b">
@@ -885,22 +855,18 @@
           <t>44751</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>53487</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="H14" t="b">
         <v>1</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Negative screening</t>
-        </is>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -949,22 +915,18 @@
           <t>65158</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>11367</t>
-        </is>
-      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Negative screening</t>
+          <t>No screening recorded</t>
         </is>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CDF demo DF stuctures fixed
</commit_message>
<xml_diff>
--- a/ccbhc_measurements/dashboard/excel files/CDF_AD_sub_1.xlsx
+++ b/ccbhc_measurements/dashboard/excel files/CDF_AD_sub_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,17 +456,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>last_encounter</t>
+          <t>numerator</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>numerator</t>
+          <t>numerator_desc</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>numerator_desc</t>
+          <t>follow_up</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -492,17 +492,19 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -522,14 +524,16 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -538,28 +542,30 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>32851-2024</t>
+          <t>26287-2024</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>32851</t>
+          <t>26287</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>58726</t>
+          <t>14630</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -568,28 +574,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>34899-2024</t>
+          <t>32851-2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>34899</t>
+          <t>32851</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>39533</t>
+          <t>58726</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -598,28 +606,30 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>35383-2024</t>
+          <t>34899-2024</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>35383</t>
+          <t>34899</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>62893</t>
+          <t>39533</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -628,28 +638,30 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>36963-2024</t>
+          <t>35383-2024</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>36963</t>
+          <t>35383</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>67362</t>
+          <t>62893</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -658,58 +670,62 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>44221-2024</t>
+          <t>36963-2024</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>44221</t>
+          <t>36963</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>64340</t>
+          <t>67362</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
       </c>
       <c r="H8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>45421-2024</t>
+          <t>44221-2024</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>45421</t>
+          <t>44221</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>26865</t>
+          <t>64340</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -718,28 +734,30 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>49143-2024</t>
+          <t>45421-2024</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>49143</t>
+          <t>45421</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>38189</t>
+          <t>26865</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -748,32 +766,30 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>56517-2024</t>
+          <t>49143-2024</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>56517</t>
+          <t>49143</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>22777</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>22777</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Negative screening</t>
-        </is>
+          <t>38189</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
       </c>
       <c r="H11" t="b">
         <v>1</v>
@@ -782,28 +798,30 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>58898-2024</t>
+          <t>56517-2024</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>58898</t>
+          <t>56517</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>93205</t>
+          <t>22777</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -812,28 +830,30 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>64017-2024</t>
+          <t>58898-2024</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>64017</t>
+          <t>58898</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>26431</t>
+          <t>93205</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -842,28 +862,30 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>76051-2024</t>
+          <t>64017-2024</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>76051</t>
+          <t>64017</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>44751</t>
+          <t>26431</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
@@ -872,28 +894,30 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>90185-2024</t>
+          <t>64607-2024</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>90185</t>
+          <t>64607</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>37034</t>
+          <t>11534</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -902,30 +926,96 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>76051-2024</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>76051</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>44751</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>90185-2024</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>90185</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>37034</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>92210-2024</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>92210</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>65158</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>No screening recorded</t>
-        </is>
-      </c>
-      <c r="H16" t="b">
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No screening recorded</t>
+        </is>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>